<commit_message>
More fixes in big database
</commit_message>
<xml_diff>
--- a/players_stats/Chris Johnson.xlsx
+++ b/players_stats/Chris Johnson.xlsx
@@ -544,17 +544,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2012-13</t>
+          <t>2010-11</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>25</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>TOT</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -564,147 +564,143 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>SF</t>
+          <t>C</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>14</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>102</t>
+          <t>138</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>9</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>21</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>.440</t>
+          <t>.429</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>.333</t>
-        </is>
-      </c>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>9</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>21</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>.714</t>
+          <t>.429</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>.560</t>
+          <t>.429</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>15</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>20</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>.500</t>
+          <t>.750</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>20</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>32</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>9</t>
         </is>
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>10</t>
         </is>
       </c>
       <c r="AD2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>21</t>
         </is>
       </c>
       <c r="AE2" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>33</t>
         </is>
       </c>
       <c r="AF2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 198</t>
+          <t xml:space="preserve"> 211</t>
         </is>
       </c>
       <c r="AG2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 93 </t>
+          <t xml:space="preserve"> 95 </t>
         </is>
       </c>
       <c r="AH2" t="inlineStr">
         <is>
-          <t>Left</t>
+          <t>Right</t>
         </is>
       </c>
       <c r="AI2" t="inlineStr"/>
@@ -715,17 +711,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2013-14</t>
+          <t>2010-11</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>25</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>POR</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -735,147 +731,143 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>SF</t>
+          <t>C</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>789</t>
+          <t>106</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>85</t>
+          <t>7</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>214</t>
+          <t>18</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>.397</t>
+          <t>.389</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>127</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>.339</t>
-        </is>
-      </c>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>7</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>87</t>
+          <t>18</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>.483</t>
+          <t>.389</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>.498</t>
+          <t>.389</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>13</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>18</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>.860</t>
+          <t>.722</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>11</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>66</t>
+          <t>16</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>97</t>
+          <t>27</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
           <t>27</t>
         </is>
       </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>63</t>
-        </is>
-      </c>
-      <c r="AE3" t="inlineStr">
-        <is>
-          <t>250</t>
-        </is>
-      </c>
       <c r="AF3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 198</t>
+          <t xml:space="preserve"> 211</t>
         </is>
       </c>
       <c r="AG3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 93 </t>
+          <t xml:space="preserve"> 95 </t>
         </is>
       </c>
       <c r="AH3" t="inlineStr">
         <is>
-          <t>Left</t>
+          <t>Right</t>
         </is>
       </c>
       <c r="AI3" t="inlineStr"/>
@@ -886,17 +878,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2014-15</t>
+          <t>2010-11</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>25</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>TOT</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -906,147 +898,143 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>SF</t>
+          <t>C</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>526</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>154</t>
+          <t>3</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>.403</t>
+          <t>.667</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>95</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>.295</t>
-        </is>
-      </c>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>2</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>59</t>
+          <t>3</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>.576</t>
+          <t>.667</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>.494</t>
+          <t>.667</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>2</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>.875</t>
+          <t>1.000</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>4</t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>5</t>
         </is>
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC4" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AD4" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AE4" t="inlineStr">
         <is>
-          <t>166</t>
+          <t>6</t>
         </is>
       </c>
       <c r="AF4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 198</t>
+          <t xml:space="preserve"> 211</t>
         </is>
       </c>
       <c r="AG4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 93 </t>
+          <t xml:space="preserve"> 95 </t>
         </is>
       </c>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>Left</t>
+          <t>Right</t>
         </is>
       </c>
       <c r="AI4" t="inlineStr"/>
@@ -1057,17 +1045,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2014-15</t>
+          <t>2011-12</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>26</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>PHI</t>
+          <t>TOT</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1077,147 +1065,143 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>SF</t>
+          <t>C</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>175</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>.488</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>.488</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>.488</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>.789</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
           <t>9</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>187</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>.317</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>.256</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>.429</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>.400</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t>.750</t>
-        </is>
-      </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="X5" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="Z5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="AA5" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="AB5" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>15</t>
         </is>
       </c>
       <c r="AD5" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>33</t>
         </is>
       </c>
       <c r="AE5" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>55</t>
         </is>
       </c>
       <c r="AF5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 198</t>
+          <t xml:space="preserve"> 211</t>
         </is>
       </c>
       <c r="AG5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 93 </t>
+          <t xml:space="preserve"> 95 </t>
         </is>
       </c>
       <c r="AH5" t="inlineStr">
         <is>
-          <t>Left</t>
+          <t>Right</t>
         </is>
       </c>
       <c r="AI5" t="inlineStr"/>
@@ -1228,17 +1212,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2014-15</t>
+          <t>2011-12</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>26</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>UTA</t>
+          <t>POR</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1248,147 +1232,143 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>SF</t>
+          <t>C</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>.478</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>.478</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>.478</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
           <t>12</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>211</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>64</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>.484</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>38</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>.342</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>.833</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
         <is>
           <t>18</t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>.692</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>.586</t>
-        </is>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>1.000</t>
-        </is>
-      </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
       <c r="Z6" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
           <t>7</t>
         </is>
       </c>
-      <c r="AA6" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="AB6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AC6" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
       <c r="AD6" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>20</t>
         </is>
       </c>
       <c r="AE6" t="inlineStr">
         <is>
-          <t>81</t>
+          <t>32</t>
         </is>
       </c>
       <c r="AF6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 198</t>
+          <t xml:space="preserve"> 211</t>
         </is>
       </c>
       <c r="AG6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 93 </t>
+          <t xml:space="preserve"> 95 </t>
         </is>
       </c>
       <c r="AH6" t="inlineStr">
         <is>
-          <t>Left</t>
+          <t>Right</t>
         </is>
       </c>
       <c r="AI6" t="inlineStr"/>
@@ -1399,17 +1379,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2014-15</t>
+          <t>2011-12</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>26</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>MIL</t>
+          <t>NOH</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1419,147 +1399,143 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>SF</t>
+          <t>C</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>.500</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>.500</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>.500</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>.714</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
           <t>8</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>128</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>.400</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>.278</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>.583</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>.483</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>1.000</t>
-        </is>
-      </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="X7" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="Y7" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="Z7" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="AA7" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="AB7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AC7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="AD7" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="AE7" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>23</t>
         </is>
       </c>
       <c r="AF7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 198</t>
+          <t xml:space="preserve"> 211</t>
         </is>
       </c>
       <c r="AG7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 93 </t>
+          <t xml:space="preserve"> 95 </t>
         </is>
       </c>
       <c r="AH7" t="inlineStr">
         <is>
-          <t>Left</t>
+          <t>Right</t>
         </is>
       </c>
       <c r="AI7" t="inlineStr"/>
@@ -1570,17 +1546,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2015-16</t>
+          <t>2012-13</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>27</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>UTA</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1590,147 +1566,143 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>SF</t>
+          <t>C</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>70</t>
+          <t>30</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>857</t>
+          <t>284</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>72</t>
+          <t>48</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>194</t>
+          <t>75</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>.371</t>
+          <t>.640</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>99</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>.273</t>
-        </is>
-      </c>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>48</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>75</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>.474</t>
+          <t>.640</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>.441</t>
+          <t>.640</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
         <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
           <t>34</t>
         </is>
       </c>
-      <c r="U8" t="inlineStr">
-        <is>
-          <t>42</t>
-        </is>
-      </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>.810</t>
+          <t>.618</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>20</t>
         </is>
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>105</t>
+          <t>40</t>
         </is>
       </c>
       <c r="Y8" t="inlineStr">
         <is>
-          <t>132</t>
+          <t>60</t>
         </is>
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>8</t>
         </is>
       </c>
       <c r="AA8" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>7</t>
         </is>
       </c>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>28</t>
         </is>
       </c>
       <c r="AC8" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>13</t>
         </is>
       </c>
       <c r="AD8" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>49</t>
         </is>
       </c>
       <c r="AE8" t="inlineStr">
         <is>
-          <t>205</t>
+          <t>117</t>
         </is>
       </c>
       <c r="AF8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 198</t>
+          <t xml:space="preserve"> 211</t>
         </is>
       </c>
       <c r="AG8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 93 </t>
+          <t xml:space="preserve"> 95 </t>
         </is>
       </c>
       <c r="AH8" t="inlineStr">
         <is>
-          <t>Left</t>
+          <t>Right</t>
         </is>
       </c>
       <c r="AI8" t="inlineStr"/>
@@ -1754,142 +1726,138 @@
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
-          <t>147</t>
+          <t>71</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>2274</t>
+          <t>597</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>230</t>
+          <t>77</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>587</t>
+          <t>137</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>.392</t>
+          <t>.562</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>104</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>339</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>.307</t>
-        </is>
-      </c>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr">
         <is>
-          <t>126</t>
+          <t>77</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>248</t>
+          <t>137</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>.508</t>
+          <t>.562</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>.480</t>
+          <t>.562</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>86</t>
+          <t>51</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
         <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>.699</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>132</t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="AD9" t="inlineStr">
+        <is>
           <t>103</t>
         </is>
       </c>
-      <c r="V9" t="inlineStr">
-        <is>
-          <t>.835</t>
-        </is>
-      </c>
-      <c r="W9" t="inlineStr">
-        <is>
-          <t>71</t>
-        </is>
-      </c>
-      <c r="X9" t="inlineStr">
-        <is>
-          <t>224</t>
-        </is>
-      </c>
-      <c r="Y9" t="inlineStr">
-        <is>
-          <t>295</t>
-        </is>
-      </c>
-      <c r="Z9" t="inlineStr">
-        <is>
-          <t>93</t>
-        </is>
-      </c>
-      <c r="AA9" t="inlineStr">
-        <is>
-          <t>89</t>
-        </is>
-      </c>
-      <c r="AB9" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
-      </c>
-      <c r="AC9" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
-      </c>
-      <c r="AD9" t="inlineStr">
-        <is>
-          <t>212</t>
-        </is>
-      </c>
       <c r="AE9" t="inlineStr">
         <is>
-          <t>650</t>
+          <t>205</t>
         </is>
       </c>
       <c r="AF9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 198</t>
+          <t xml:space="preserve"> 211</t>
         </is>
       </c>
       <c r="AG9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 93 </t>
+          <t xml:space="preserve"> 95 </t>
         </is>
       </c>
       <c r="AH9" t="inlineStr">
         <is>
-          <t>Left</t>
+          <t>Right</t>
         </is>
       </c>
       <c r="AI9" t="inlineStr"/>

</xml_diff>